<commit_message>
Typo of Manufacturer Part Number
</commit_message>
<xml_diff>
--- a/biosignal-daq-v1.0-bom.xlsx
+++ b/biosignal-daq-v1.0-bom.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dewald/Documents/eagle/Biosignal DAQ V1.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Slåttnes\Documents\GitHub\Biosignal-DAQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{696CA35A-1105-D84E-8D9C-99B666A96898}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A61C08C-9595-4727-9B59-8B7EB9E02E3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="3300" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="2400" yWindow="3300" windowWidth="27636" windowHeight="16944" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="biosignal-daq-v1.0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -364,9 +364,6 @@
     <t>KEMET</t>
   </si>
   <si>
-    <t>MCWR06W47R0FTL</t>
-  </si>
-  <si>
     <t>0603N561J500CT</t>
   </si>
   <si>
@@ -398,12 +395,15 @@
   </si>
   <si>
     <t>CUI</t>
+  </si>
+  <si>
+    <t>MCWR06X47R0FTL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -944,22 +944,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J31" totalsRowCount="1">
-  <autoFilter ref="A2:J30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:J31" totalsRowCount="1">
+  <autoFilter ref="A2:J30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A3:J30">
     <sortCondition ref="E2:E30"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="Qty" totalsRowFunction="sum"/>
-    <tableColumn id="2" name="Value"/>
-    <tableColumn id="3" name="Device"/>
-    <tableColumn id="4" name="Package"/>
-    <tableColumn id="5" name="Parts"/>
-    <tableColumn id="7" name="MANUFACTURER_PART_NUMBER"/>
-    <tableColumn id="9" name="RATING"/>
-    <tableColumn id="11" name="TECHNOLOGY"/>
-    <tableColumn id="12" name="TOLERANCE"/>
-    <tableColumn id="14" name="VENDOR"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Qty" totalsRowFunction="sum"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Device"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Package"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parts"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="MANUFACTURER_PART_NUMBER"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="RATING"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="TECHNOLOGY"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="TOLERANCE"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="VENDOR"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1261,27 +1261,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" customWidth="1"/>
+    <col min="9" max="9" width="13.296875" customWidth="1"/>
+    <col min="10" max="10" width="16.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>9</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>11</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>11</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1551,10 +1551,10 @@
         <v>58</v>
       </c>
       <c r="F10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" t="s">
         <v>115</v>
-      </c>
-      <c r="G10" t="s">
-        <v>116</v>
       </c>
       <c r="H10" t="s">
         <v>90</v>
@@ -1566,7 +1566,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1635,10 +1635,10 @@
         <v>33</v>
       </c>
       <c r="E13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" t="s">
         <v>117</v>
-      </c>
-      <c r="F13" t="s">
-        <v>118</v>
       </c>
       <c r="G13" t="s">
         <v>40</v>
@@ -1650,7 +1650,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="G18" t="s">
         <v>100</v>
@@ -1795,7 +1795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G20" t="s">
         <v>100</v>
@@ -1853,7 +1853,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G22" t="s">
         <v>100</v>
@@ -1911,7 +1911,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1928,13 +1928,13 @@
         <v>63</v>
       </c>
       <c r="F23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1997,13 +1997,13 @@
         <v>81</v>
       </c>
       <c r="F26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -2089,13 +2089,13 @@
         <v>84</v>
       </c>
       <c r="F30" t="s">
+        <v>123</v>
+      </c>
+      <c r="J30" t="s">
         <v>124</v>
       </c>
-      <c r="J30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <f>SUBTOTAL(109,Table1[Qty])</f>
         <v>129</v>

</xml_diff>